<commit_message>
CCH4, NN2O and CCO2 Gasera transformations in Master_GHG_2023
</commit_message>
<xml_diff>
--- a/outputs/CERESTRES_results/Gasera_vs_Chromat/Master_CON_GS_CH4.xlsx
+++ b/outputs/CERESTRES_results/Gasera_vs_Chromat/Master_CON_GS_CH4.xlsx
@@ -377,12 +377,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>avg_Gasera_CH4_flux_mgm2h</t>
+          <t>avg_Gasera_CCH4_flux_mgm2h</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>avg_Gasera_CH4_flux_mgm2h_cor</t>
+          <t>avg_Gasera_CCH4_flux_mgm2h_cor</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -401,10 +401,10 @@
         </is>
       </c>
       <c r="C2">
-        <v>-0.942521999141831</v>
+        <v>-0.53016862451728</v>
       </c>
       <c r="D2">
-        <v>-0.9956141953299409</v>
+        <v>-0.5600329848730917</v>
       </c>
       <c r="E2">
         <v>-0.06081587914173636</v>
@@ -420,10 +420,10 @@
         </is>
       </c>
       <c r="C3">
-        <v>3.928696001859111</v>
+        <v>2.20989150104575</v>
       </c>
       <c r="D3">
-        <v>3.762238010078355</v>
+        <v>2.116258880669075</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -439,10 +439,10 @@
         </is>
       </c>
       <c r="C4">
-        <v>0.7692628121748122</v>
+        <v>0.4327103318483319</v>
       </c>
       <c r="D4">
-        <v>1.012827899227072</v>
+        <v>0.569715693315228</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="C5">
-        <v>2.032071518380267</v>
+        <v>1.1430402290889</v>
       </c>
       <c r="D5">
-        <v>2.502046637359297</v>
+        <v>1.407401233514605</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -477,10 +477,10 @@
         </is>
       </c>
       <c r="C6">
-        <v>1.46981362665185</v>
+        <v>0.8267701649916656</v>
       </c>
       <c r="D6">
-        <v>1.668181989235994</v>
+        <v>0.9383523689452468</v>
       </c>
       <c r="E6">
         <v>0.06415260808324212</v>
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="C7">
-        <v>0.5678672562547279</v>
+        <v>0.3194253316432845</v>
       </c>
       <c r="D7">
-        <v>0.4647419445618057</v>
+        <v>0.2614173438160157</v>
       </c>
       <c r="E7">
         <v>0.1388286885926989</v>
@@ -515,10 +515,10 @@
         </is>
       </c>
       <c r="C8">
-        <v>-3.297427553008139</v>
+        <v>-1.854802998567078</v>
       </c>
       <c r="D8">
-        <v>-2.789362361344979</v>
+        <v>-1.569016328256551</v>
       </c>
       <c r="E8">
         <v>0.2234246157778144</v>
@@ -534,10 +534,10 @@
         </is>
       </c>
       <c r="C9">
-        <v>-3.090987479238966</v>
+        <v>-1.738680457071919</v>
       </c>
       <c r="D9">
-        <v>-3.090987479238966</v>
+        <v>-1.738680457071919</v>
       </c>
       <c r="E9">
         <v>0.5210128514309061</v>
@@ -553,7 +553,7 @@
         </is>
       </c>
       <c r="C10">
-        <v>0.9499781831510327</v>
+        <v>0.5343627280224559</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="C11">
-        <v>1.528290871827222</v>
+        <v>0.8596636154028126</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="C12">
-        <v>-0.2925624123479318</v>
+        <v>-0.1645663569457116</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -610,10 +610,10 @@
         </is>
       </c>
       <c r="C13">
-        <v>1.238989405548146</v>
+        <v>0.6969315406208321</v>
       </c>
       <c r="D13">
-        <v>1.554700191104661</v>
+        <v>0.8745188574963721</v>
       </c>
       <c r="E13">
         <v>2.172942224685735</v>
@@ -629,10 +629,10 @@
         </is>
       </c>
       <c r="C14">
-        <v>1.197007064276813</v>
+        <v>0.6733164736557071</v>
       </c>
       <c r="D14">
-        <v>1.638792844858032</v>
+        <v>0.9218209752326431</v>
       </c>
       <c r="E14">
         <v>3.270392275133001</v>
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="C15">
-        <v>-0.992852052092834</v>
+        <v>-0.5584792793022191</v>
       </c>
       <c r="D15">
-        <v>-0.7624578058339305</v>
+        <v>-0.4288825157815859</v>
       </c>
       <c r="E15">
         <v>3.946377750758421</v>
@@ -667,10 +667,10 @@
         </is>
       </c>
       <c r="C16">
-        <v>2.464329069965655</v>
+        <v>1.386185101855681</v>
       </c>
       <c r="D16">
-        <v>2.200205774572355</v>
+        <v>1.23761574819695</v>
       </c>
       <c r="E16">
         <v>4.437161647424185</v>
@@ -686,10 +686,10 @@
         </is>
       </c>
       <c r="C17">
-        <v>4.609183693315479</v>
+        <v>2.592665827489957</v>
       </c>
       <c r="D17">
-        <v>4.609183693315479</v>
+        <v>2.592665827489957</v>
       </c>
       <c r="E17">
         <v>5.555564497453742</v>
@@ -705,10 +705,10 @@
         </is>
       </c>
       <c r="C18">
-        <v>2.032195326557931</v>
+        <v>1.143109871188836</v>
       </c>
       <c r="D18">
-        <v>1.719514331101512</v>
+        <v>0.9672268112446004</v>
       </c>
       <c r="E18">
         <v>6.608357174397154</v>

</xml_diff>